<commit_message>
filling NANs in inputs.
</commit_message>
<xml_diff>
--- a/All_Channel_Inputs.xlsx
+++ b/All_Channel_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\2023\Nestle CPW\Python Workflows\Blueprint DB Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2191C0A-E5B8-403F-9930-C4329D1E70A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080244AA-4F9F-4F03-916D-CE40650C99F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1021,7 +1021,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1089,7 +1089,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1393,25 +1393,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F189" sqref="F189"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="K190" sqref="K190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1463,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1570,7 +1569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1623,7 +1622,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1676,7 +1675,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1782,7 +1781,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1835,7 +1834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1888,7 +1887,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1941,7 +1940,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2047,7 +2046,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2100,7 +2099,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2153,7 +2152,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2312,7 +2311,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2365,7 +2364,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2468,7 +2467,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2568,7 +2567,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2618,7 +2617,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2668,7 +2667,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2718,7 +2717,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2818,7 +2817,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2868,7 +2867,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2968,7 +2967,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3018,7 +3017,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3068,7 +3067,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3118,7 +3117,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3168,7 +3167,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3218,7 +3217,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3268,7 +3267,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3318,7 +3317,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3368,7 +3367,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3418,7 +3417,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3468,7 +3467,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3518,7 +3517,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3568,7 +3567,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3618,7 +3617,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3668,7 +3667,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3718,7 +3717,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3768,7 +3767,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3818,7 +3817,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3868,7 +3867,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3918,7 +3917,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3968,7 +3967,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4018,7 +4017,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4068,7 +4067,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4118,7 +4117,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4168,7 +4167,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4218,7 +4217,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4268,7 +4267,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4318,7 +4317,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4368,7 +4367,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4418,7 +4417,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4468,7 +4467,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4518,7 +4517,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4568,7 +4567,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4618,7 +4617,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4668,7 +4667,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4718,7 +4717,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4768,7 +4767,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4818,7 +4817,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4868,7 +4867,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4918,7 +4917,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4968,7 +4967,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -5018,7 +5017,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -5068,7 +5067,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -5118,7 +5117,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -5168,7 +5167,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -5218,7 +5217,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -5268,7 +5267,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -5318,7 +5317,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -5368,7 +5367,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -5418,7 +5417,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -5468,7 +5467,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -5518,7 +5517,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -5568,7 +5567,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -5618,7 +5617,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -5668,7 +5667,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -5718,7 +5717,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="86" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -5768,7 +5767,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -5818,7 +5817,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -5868,7 +5867,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -5918,7 +5917,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -5968,7 +5967,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -6018,7 +6017,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -6068,7 +6067,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="93" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -6118,7 +6117,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -6168,7 +6167,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -6218,7 +6217,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -6268,7 +6267,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -6318,7 +6317,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -6368,7 +6367,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -6418,7 +6417,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -6468,7 +6467,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
@@ -6518,7 +6517,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
@@ -6568,7 +6567,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>101</v>
       </c>
@@ -6618,7 +6617,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>102</v>
       </c>
@@ -6668,7 +6667,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103</v>
       </c>
@@ -6718,7 +6717,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>104</v>
       </c>
@@ -6768,7 +6767,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>105</v>
       </c>
@@ -6818,7 +6817,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>106</v>
       </c>
@@ -6868,7 +6867,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107</v>
       </c>
@@ -6918,7 +6917,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>108</v>
       </c>
@@ -6968,7 +6967,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>109</v>
       </c>
@@ -7018,7 +7017,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>110</v>
       </c>
@@ -7068,7 +7067,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>111</v>
       </c>
@@ -7118,7 +7117,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>112</v>
       </c>
@@ -7168,7 +7167,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>113</v>
       </c>
@@ -7218,7 +7217,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>114</v>
       </c>
@@ -7268,7 +7267,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>115</v>
       </c>
@@ -7318,7 +7317,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>116</v>
       </c>
@@ -7368,7 +7367,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>117</v>
       </c>
@@ -7418,7 +7417,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>118</v>
       </c>
@@ -7468,7 +7467,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="121" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>119</v>
       </c>
@@ -7518,7 +7517,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="122" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>120</v>
       </c>
@@ -7568,7 +7567,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="123" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>121</v>
       </c>
@@ -7618,7 +7617,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="124" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>122</v>
       </c>
@@ -7668,7 +7667,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="125" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>123</v>
       </c>
@@ -7721,7 +7720,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="126" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>124</v>
       </c>
@@ -7774,7 +7773,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>125</v>
       </c>
@@ -7827,7 +7826,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="128" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>126</v>
       </c>
@@ -7880,7 +7879,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="129" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>127</v>
       </c>
@@ -7933,7 +7932,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="130" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>128</v>
       </c>
@@ -7986,7 +7985,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>129</v>
       </c>
@@ -8039,7 +8038,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="132" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>130</v>
       </c>
@@ -8092,7 +8091,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="133" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>131</v>
       </c>
@@ -8145,7 +8144,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>132</v>
       </c>
@@ -8198,7 +8197,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>133</v>
       </c>
@@ -8251,7 +8250,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="136" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>134</v>
       </c>
@@ -8304,7 +8303,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="137" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>135</v>
       </c>
@@ -8354,7 +8353,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="138" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>136</v>
       </c>
@@ -8404,7 +8403,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="139" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>137</v>
       </c>
@@ -8454,7 +8453,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="140" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>138</v>
       </c>
@@ -8504,7 +8503,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>139</v>
       </c>
@@ -8554,7 +8553,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="142" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>140</v>
       </c>
@@ -8604,7 +8603,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>141</v>
       </c>
@@ -8654,7 +8653,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>142</v>
       </c>
@@ -8704,7 +8703,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="145" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>143</v>
       </c>
@@ -8754,7 +8753,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>144</v>
       </c>
@@ -8804,7 +8803,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>145</v>
       </c>
@@ -8854,7 +8853,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="148" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>146</v>
       </c>
@@ -8904,7 +8903,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="149" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>147</v>
       </c>
@@ -8954,7 +8953,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="150" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>148</v>
       </c>
@@ -9004,7 +9003,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>149</v>
       </c>
@@ -9054,7 +9053,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="152" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>150</v>
       </c>
@@ -9104,7 +9103,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>151</v>
       </c>
@@ -9154,7 +9153,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="154" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>152</v>
       </c>
@@ -9204,7 +9203,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="155" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>153</v>
       </c>
@@ -9254,7 +9253,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>154</v>
       </c>
@@ -9304,7 +9303,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="157" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>155</v>
       </c>
@@ -9354,7 +9353,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="158" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>156</v>
       </c>
@@ -9404,7 +9403,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="159" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>157</v>
       </c>
@@ -9454,7 +9453,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>158</v>
       </c>
@@ -9504,7 +9503,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="161" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>159</v>
       </c>
@@ -9554,7 +9553,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="162" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>160</v>
       </c>
@@ -9604,7 +9603,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="163" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>161</v>
       </c>
@@ -9654,7 +9653,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>162</v>
       </c>
@@ -9704,7 +9703,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>163</v>
       </c>
@@ -9754,7 +9753,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="166" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>164</v>
       </c>
@@ -9804,7 +9803,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="167" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>165</v>
       </c>
@@ -9854,7 +9853,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="168" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>166</v>
       </c>
@@ -9904,7 +9903,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>167</v>
       </c>
@@ -9954,7 +9953,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>168</v>
       </c>
@@ -10004,7 +10003,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="171" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>169</v>
       </c>
@@ -10054,7 +10053,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>170</v>
       </c>
@@ -10104,7 +10103,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="173" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>171</v>
       </c>
@@ -10154,7 +10153,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>172</v>
       </c>
@@ -10204,7 +10203,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="175" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>173</v>
       </c>
@@ -10254,7 +10253,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>174</v>
       </c>
@@ -10304,7 +10303,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="177" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>175</v>
       </c>
@@ -10354,7 +10353,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>176</v>
       </c>
@@ -10404,7 +10403,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="179" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>177</v>
       </c>
@@ -10454,7 +10453,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="180" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -10504,7 +10503,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -10541,11 +10540,20 @@
       <c r="L181">
         <v>1.1604548212938649E-3</v>
       </c>
+      <c r="N181">
+        <v>0</v>
+      </c>
+      <c r="O181">
+        <v>0</v>
+      </c>
+      <c r="P181">
+        <v>0</v>
+      </c>
       <c r="Q181" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -10582,11 +10590,20 @@
       <c r="L182">
         <v>0.54072400773841567</v>
       </c>
+      <c r="N182">
+        <v>0</v>
+      </c>
+      <c r="O182">
+        <v>0</v>
+      </c>
+      <c r="P182">
+        <v>0</v>
+      </c>
       <c r="Q182" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -10623,11 +10640,20 @@
       <c r="L183">
         <v>1.00818285693965E-2</v>
       </c>
+      <c r="N183">
+        <v>0</v>
+      </c>
+      <c r="O183">
+        <v>0</v>
+      </c>
+      <c r="P183">
+        <v>0</v>
+      </c>
       <c r="Q183" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -10664,11 +10690,20 @@
       <c r="L184">
         <v>0.55698737026565415</v>
       </c>
+      <c r="N184">
+        <v>0</v>
+      </c>
+      <c r="O184">
+        <v>0</v>
+      </c>
+      <c r="P184">
+        <v>0</v>
+      </c>
       <c r="Q184" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
@@ -10705,11 +10740,20 @@
       <c r="L185">
         <v>0.20875208025856121</v>
       </c>
+      <c r="N185">
+        <v>0</v>
+      </c>
+      <c r="O185">
+        <v>0</v>
+      </c>
+      <c r="P185">
+        <v>0</v>
+      </c>
       <c r="Q185" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
@@ -10746,11 +10790,20 @@
       <c r="L186">
         <v>3.49840256698588E-3</v>
       </c>
+      <c r="N186">
+        <v>0</v>
+      </c>
+      <c r="O186">
+        <v>0</v>
+      </c>
+      <c r="P186">
+        <v>0</v>
+      </c>
       <c r="Q186" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
@@ -10787,11 +10840,20 @@
       <c r="L187">
         <v>0.73696567510388022</v>
       </c>
+      <c r="N187">
+        <v>0</v>
+      </c>
+      <c r="O187">
+        <v>0</v>
+      </c>
+      <c r="P187">
+        <v>0</v>
+      </c>
       <c r="Q187" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
@@ -10828,18 +10890,21 @@
       <c r="L188">
         <v>0.20349046478957361</v>
       </c>
+      <c r="N188">
+        <v>0</v>
+      </c>
+      <c r="O188">
+        <v>0</v>
+      </c>
+      <c r="P188">
+        <v>0</v>
+      </c>
       <c r="Q188" t="s">
         <v>324</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q188" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="KitKat"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q188" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>